<commit_message>
add new sequences and cue creation script
</commit_message>
<xml_diff>
--- a/sequences/01_retrieval_1.xlsx
+++ b/sequences/01_retrieval_1.xlsx
@@ -1051,385 +1051,385 @@
     <t>face/face212.jpg</t>
   </si>
   <si>
+    <t>face/face259.jpg</t>
+  </si>
+  <si>
+    <t>face/face245.jpg</t>
+  </si>
+  <si>
+    <t>house/house210.jpg</t>
+  </si>
+  <si>
+    <t>face/face158.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog099.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower174.jpg</t>
+  </si>
+  <si>
+    <t>house/house109.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower216.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower207.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog150.jpg</t>
+  </si>
+  <si>
+    <t>face/face108.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog256.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower238.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower130.jpg</t>
+  </si>
+  <si>
+    <t>face/face186.jpg</t>
+  </si>
+  <si>
+    <t>face/face207.jpg</t>
+  </si>
+  <si>
+    <t>face/face229.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog203.jpg</t>
+  </si>
+  <si>
+    <t>house/house208.jpg</t>
+  </si>
+  <si>
+    <t>house/house130.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog257.jpg</t>
+  </si>
+  <si>
+    <t>face/face149.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower196.jpg</t>
+  </si>
+  <si>
+    <t>face/face228.jpg</t>
+  </si>
+  <si>
+    <t>house/house151.jpg</t>
+  </si>
+  <si>
+    <t>face/face102.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower260.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog155.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower235.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower232.jpg</t>
+  </si>
+  <si>
+    <t>house/house097.jpg</t>
+  </si>
+  <si>
+    <t>house/house152.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower129.jpg</t>
+  </si>
+  <si>
+    <t>face/face164.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower204.jpg</t>
+  </si>
+  <si>
+    <t>face/face213.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog199.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog114.jpg</t>
+  </si>
+  <si>
+    <t>house/house120.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower162.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower248.jpg</t>
+  </si>
+  <si>
+    <t>face/face225.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog263.jpg</t>
+  </si>
+  <si>
+    <t>face/face178.jpg</t>
+  </si>
+  <si>
+    <t>house/house238.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog252.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog144.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog135.jpg</t>
+  </si>
+  <si>
+    <t>house/house209.jpg</t>
+  </si>
+  <si>
+    <t>house/house195.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower109.jpg</t>
+  </si>
+  <si>
+    <t>face/face235.jpg</t>
+  </si>
+  <si>
+    <t>face/face249.jpg</t>
+  </si>
+  <si>
+    <t>house/house244.jpg</t>
+  </si>
+  <si>
+    <t>house/house126.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog152.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower131.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower186.jpg</t>
+  </si>
+  <si>
+    <t>face/face214.jpg</t>
+  </si>
+  <si>
+    <t>face/face103.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower218.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower258.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog149.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog185.jpg</t>
+  </si>
+  <si>
+    <t>house/house198.jpg</t>
+  </si>
+  <si>
+    <t>face/face227.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower250.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog243.jpg</t>
+  </si>
+  <si>
     <t>house/house193.jpg</t>
   </si>
   <si>
+    <t>house/house168.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower185.jpg</t>
+  </si>
+  <si>
+    <t>house/house137.jpg</t>
+  </si>
+  <si>
+    <t>house/house112.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower120.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower127.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower223.jpg</t>
+  </si>
+  <si>
+    <t>house/house257.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog190.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog103.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower236.jpg</t>
+  </si>
+  <si>
+    <t>house/house245.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog151.jpg</t>
+  </si>
+  <si>
+    <t>face/face209.jpg</t>
+  </si>
+  <si>
+    <t>face/face130.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower141.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog200.jpg</t>
+  </si>
+  <si>
+    <t>house/house202.jpg</t>
+  </si>
+  <si>
+    <t>house/house164.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower152.jpg</t>
+  </si>
+  <si>
+    <t>face/face113.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower142.jpg</t>
+  </si>
+  <si>
+    <t>house/house107.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower153.jpg</t>
+  </si>
+  <si>
+    <t>house/house263.jpg</t>
+  </si>
+  <si>
+    <t>face/face216.jpg</t>
+  </si>
+  <si>
+    <t>house/house138.jpg</t>
+  </si>
+  <si>
+    <t>house/house221.jpg</t>
+  </si>
+  <si>
+    <t>face/face140.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog174.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog198.jpg</t>
+  </si>
+  <si>
+    <t>house/house236.jpg</t>
+  </si>
+  <si>
     <t>face/face185.jpg</t>
   </si>
   <si>
-    <t>face/face235.jpg</t>
-  </si>
-  <si>
-    <t>house/house152.jpg</t>
-  </si>
-  <si>
-    <t>face/face228.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog103.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog257.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower216.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog243.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower141.jpg</t>
-  </si>
-  <si>
-    <t>face/face158.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower131.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower238.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower196.jpg</t>
-  </si>
-  <si>
-    <t>house/house257.jpg</t>
-  </si>
-  <si>
-    <t>house/house245.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog185.jpg</t>
-  </si>
-  <si>
-    <t>house/house209.jpg</t>
-  </si>
-  <si>
-    <t>house/house195.jpg</t>
-  </si>
-  <si>
-    <t>face/face227.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog256.jpg</t>
-  </si>
-  <si>
-    <t>house/house097.jpg</t>
-  </si>
-  <si>
-    <t>face/face249.jpg</t>
-  </si>
-  <si>
-    <t>face/face113.jpg</t>
-  </si>
-  <si>
-    <t>face/face207.jpg</t>
+    <t>house/house170.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog161.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog241.jpg</t>
+  </si>
+  <si>
+    <t>face/face162.jpg</t>
+  </si>
+  <si>
+    <t>house/house132.jpg</t>
+  </si>
+  <si>
+    <t>house/house158.jpg</t>
+  </si>
+  <si>
+    <t>house/house227.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog244.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog132.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower111.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog112.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog207.jpg</t>
+  </si>
+  <si>
+    <t>face/face233.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog245.jpg</t>
   </si>
   <si>
     <t>face/face195.jpg</t>
   </si>
   <si>
-    <t>flower/flower236.jpg</t>
-  </si>
-  <si>
-    <t>house/house227.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower111.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower232.jpg</t>
+    <t>flower/flower168.jpg</t>
+  </si>
+  <si>
+    <t>face/face192.jpg</t>
+  </si>
+  <si>
+    <t>face/face250.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog229.jpg</t>
+  </si>
+  <si>
+    <t>dog/dog195.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower193.jpg</t>
+  </si>
+  <si>
+    <t>face/face194.jpg</t>
+  </si>
+  <si>
+    <t>house/house251.jpg</t>
+  </si>
+  <si>
+    <t>flower/flower146.jpg</t>
   </si>
   <si>
     <t>dog/dog253.jpg</t>
-  </si>
-  <si>
-    <t>face/face108.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower248.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog245.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog132.jpg</t>
-  </si>
-  <si>
-    <t>house/house210.jpg</t>
-  </si>
-  <si>
-    <t>face/face250.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog151.jpg</t>
-  </si>
-  <si>
-    <t>house/house138.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower162.jpg</t>
-  </si>
-  <si>
-    <t>face/face149.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog195.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog150.jpg</t>
-  </si>
-  <si>
-    <t>house/house244.jpg</t>
-  </si>
-  <si>
-    <t>face/face259.jpg</t>
-  </si>
-  <si>
-    <t>face/face162.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower146.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog155.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog203.jpg</t>
-  </si>
-  <si>
-    <t>face/face103.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower235.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower109.jpg</t>
-  </si>
-  <si>
-    <t>house/house158.jpg</t>
-  </si>
-  <si>
-    <t>face/face213.jpg</t>
-  </si>
-  <si>
-    <t>house/house221.jpg</t>
-  </si>
-  <si>
-    <t>house/house164.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower250.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower186.jpg</t>
-  </si>
-  <si>
-    <t>house/house251.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog199.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower218.jpg</t>
-  </si>
-  <si>
-    <t>house/house151.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog099.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog198.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog174.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog207.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower127.jpg</t>
-  </si>
-  <si>
-    <t>face/face102.jpg</t>
-  </si>
-  <si>
-    <t>house/house120.jpg</t>
-  </si>
-  <si>
-    <t>face/face245.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog114.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog152.jpg</t>
-  </si>
-  <si>
-    <t>face/face140.jpg</t>
-  </si>
-  <si>
-    <t>house/house198.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower174.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower223.jpg</t>
-  </si>
-  <si>
-    <t>face/face186.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog241.jpg</t>
-  </si>
-  <si>
-    <t>house/house112.jpg</t>
-  </si>
-  <si>
-    <t>house/house130.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower260.jpg</t>
-  </si>
-  <si>
-    <t>face/face194.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower120.jpg</t>
-  </si>
-  <si>
-    <t>house/house126.jpg</t>
-  </si>
-  <si>
-    <t>face/face192.jpg</t>
-  </si>
-  <si>
-    <t>face/face216.jpg</t>
-  </si>
-  <si>
-    <t>face/face214.jpg</t>
-  </si>
-  <si>
-    <t>house/house137.jpg</t>
-  </si>
-  <si>
-    <t>face/face233.jpg</t>
-  </si>
-  <si>
-    <t>house/house107.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog135.jpg</t>
-  </si>
-  <si>
-    <t>house/house263.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog144.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog149.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower152.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog161.jpg</t>
-  </si>
-  <si>
-    <t>face/face164.jpg</t>
-  </si>
-  <si>
-    <t>house/house109.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog190.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower258.jpg</t>
-  </si>
-  <si>
-    <t>house/house170.jpg</t>
-  </si>
-  <si>
-    <t>house/house168.jpg</t>
-  </si>
-  <si>
-    <t>face/face178.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog229.jpg</t>
-  </si>
-  <si>
-    <t>face/face209.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower130.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog200.jpg</t>
-  </si>
-  <si>
-    <t>house/house238.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog252.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog244.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower204.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog263.jpg</t>
-  </si>
-  <si>
-    <t>house/house236.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower153.jpg</t>
-  </si>
-  <si>
-    <t>house/house202.jpg</t>
-  </si>
-  <si>
-    <t>house/house208.jpg</t>
-  </si>
-  <si>
-    <t>face/face225.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower168.jpg</t>
-  </si>
-  <si>
-    <t>house/house132.jpg</t>
-  </si>
-  <si>
-    <t>face/face130.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower185.jpg</t>
-  </si>
-  <si>
-    <t>dog/dog112.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower207.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower142.jpg</t>
-  </si>
-  <si>
-    <t>face/face229.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower193.jpg</t>
-  </si>
-  <si>
-    <t>flower/flower129.jpg</t>
   </si>
   <si>
     <t>other/old/uncued</t>
@@ -1890,7 +1890,7 @@
         <v>298</v>
       </c>
       <c r="H2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="I2" t="s">
         <v>344</v>
@@ -1899,7 +1899,7 @@
         <v>343</v>
       </c>
       <c r="K2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="L2" t="s">
         <v>472</v>
@@ -1949,13 +1949,13 @@
         <v>245</v>
       </c>
       <c r="H3" t="s">
-        <v>336</v>
+        <v>250</v>
       </c>
       <c r="I3" t="s">
         <v>345</v>
       </c>
       <c r="J3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K3" t="s">
         <v>345</v>
@@ -1970,7 +1970,7 @@
         <v>474</v>
       </c>
       <c r="O3" t="s">
-        <v>336</v>
+        <v>250</v>
       </c>
       <c r="P3" t="s">
         <v>472</v>
@@ -2126,7 +2126,7 @@
         <v>271</v>
       </c>
       <c r="H6" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="I6" t="s">
         <v>346</v>
@@ -2153,7 +2153,7 @@
         <v>475</v>
       </c>
       <c r="Q6" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="R6" t="s">
         <v>472</v>
@@ -2185,13 +2185,13 @@
         <v>338</v>
       </c>
       <c r="H7" t="s">
-        <v>233</v>
+        <v>295</v>
       </c>
       <c r="I7" t="s">
         <v>347</v>
       </c>
       <c r="J7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K7" t="s">
         <v>347</v>
@@ -2212,7 +2212,7 @@
         <v>475</v>
       </c>
       <c r="Q7" t="s">
-        <v>233</v>
+        <v>295</v>
       </c>
       <c r="R7" t="s">
         <v>472</v>
@@ -2303,13 +2303,13 @@
         <v>310</v>
       </c>
       <c r="H9" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="I9" t="s">
         <v>348</v>
       </c>
       <c r="J9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K9" t="s">
         <v>310</v>
@@ -2324,7 +2324,7 @@
         <v>473</v>
       </c>
       <c r="O9" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="P9" t="s">
         <v>472</v>
@@ -2362,13 +2362,13 @@
         <v>296</v>
       </c>
       <c r="H10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I10" t="s">
         <v>349</v>
       </c>
       <c r="J10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K10" t="s">
         <v>217</v>
@@ -2389,7 +2389,7 @@
         <v>473</v>
       </c>
       <c r="Q10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="R10" t="s">
         <v>472</v>
@@ -2471,25 +2471,25 @@
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>218</v>
       </c>
       <c r="G12" t="s">
-        <v>332</v>
+        <v>238</v>
       </c>
       <c r="H12" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="I12" t="s">
         <v>350</v>
       </c>
       <c r="J12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K12" t="s">
-        <v>332</v>
+        <v>238</v>
       </c>
       <c r="L12" t="s">
         <v>475</v>
@@ -2501,7 +2501,7 @@
         <v>473</v>
       </c>
       <c r="O12" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="P12" t="s">
         <v>472</v>
@@ -2510,7 +2510,7 @@
         <v>218</v>
       </c>
       <c r="R12" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S12">
         <v>1.134775852873516</v>
@@ -2530,22 +2530,22 @@
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>219</v>
       </c>
       <c r="G13" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="H13" t="s">
-        <v>330</v>
+        <v>249</v>
       </c>
       <c r="I13" t="s">
         <v>351</v>
       </c>
       <c r="J13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K13" t="s">
         <v>351</v>
@@ -2554,13 +2554,13 @@
         <v>473</v>
       </c>
       <c r="M13" t="s">
-        <v>330</v>
+        <v>249</v>
       </c>
       <c r="N13" t="s">
         <v>472</v>
       </c>
       <c r="O13" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="P13" t="s">
         <v>475</v>
@@ -2569,7 +2569,7 @@
         <v>219</v>
       </c>
       <c r="R13" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S13">
         <v>1.115037862213843</v>
@@ -2589,16 +2589,16 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>220</v>
       </c>
       <c r="G14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H14" t="s">
-        <v>317</v>
+        <v>251</v>
       </c>
       <c r="I14" t="s">
         <v>352</v>
@@ -2607,13 +2607,13 @@
         <v>340</v>
       </c>
       <c r="K14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L14" t="s">
         <v>475</v>
       </c>
       <c r="M14" t="s">
-        <v>317</v>
+        <v>251</v>
       </c>
       <c r="N14" t="s">
         <v>472</v>
@@ -2628,7 +2628,7 @@
         <v>220</v>
       </c>
       <c r="R14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S14">
         <v>1.149190243648563</v>
@@ -2648,25 +2648,25 @@
         <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>221</v>
       </c>
       <c r="G15" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="H15" t="s">
-        <v>338</v>
+        <v>258</v>
       </c>
       <c r="I15" t="s">
         <v>353</v>
       </c>
       <c r="J15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K15" t="s">
-        <v>338</v>
+        <v>258</v>
       </c>
       <c r="L15" t="s">
         <v>472</v>
@@ -2675,10 +2675,10 @@
         <v>221</v>
       </c>
       <c r="N15" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O15" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="P15" t="s">
         <v>475</v>
@@ -2766,22 +2766,22 @@
         <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>222</v>
       </c>
       <c r="G17" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="H17" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="I17" t="s">
         <v>354</v>
       </c>
       <c r="J17" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K17" t="s">
         <v>354</v>
@@ -2790,13 +2790,13 @@
         <v>473</v>
       </c>
       <c r="M17" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="N17" t="s">
         <v>475</v>
       </c>
       <c r="O17" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="P17" t="s">
         <v>472</v>
@@ -2805,7 +2805,7 @@
         <v>222</v>
       </c>
       <c r="R17" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S17">
         <v>1.006233008272824</v>
@@ -2825,16 +2825,16 @@
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>223</v>
       </c>
       <c r="G18" t="s">
-        <v>249</v>
+        <v>326</v>
       </c>
       <c r="H18" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="I18" t="s">
         <v>355</v>
@@ -2843,7 +2843,7 @@
         <v>343</v>
       </c>
       <c r="K18" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="L18" t="s">
         <v>472</v>
@@ -2852,10 +2852,10 @@
         <v>223</v>
       </c>
       <c r="N18" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O18" t="s">
-        <v>249</v>
+        <v>326</v>
       </c>
       <c r="P18" t="s">
         <v>475</v>
@@ -2884,31 +2884,31 @@
         <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>224</v>
       </c>
       <c r="G19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H19" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
       <c r="I19" t="s">
         <v>356</v>
       </c>
       <c r="J19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L19" t="s">
         <v>475</v>
       </c>
       <c r="M19" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
       <c r="N19" t="s">
         <v>472</v>
@@ -2923,7 +2923,7 @@
         <v>224</v>
       </c>
       <c r="R19" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S19">
         <v>1.092158232689251</v>
@@ -3188,13 +3188,13 @@
         <v>309</v>
       </c>
       <c r="H24" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="I24" t="s">
         <v>359</v>
       </c>
       <c r="J24" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K24" t="s">
         <v>359</v>
@@ -3209,7 +3209,7 @@
         <v>475</v>
       </c>
       <c r="O24" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="P24" t="s">
         <v>472</v>
@@ -3247,13 +3247,13 @@
         <v>234</v>
       </c>
       <c r="H25" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="I25" t="s">
         <v>360</v>
       </c>
       <c r="J25" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K25" t="s">
         <v>360</v>
@@ -3274,7 +3274,7 @@
         <v>474</v>
       </c>
       <c r="Q25" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="R25" t="s">
         <v>472</v>
@@ -3365,13 +3365,13 @@
         <v>251</v>
       </c>
       <c r="H27" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="I27" t="s">
         <v>361</v>
       </c>
       <c r="J27" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="K27" t="s">
         <v>361</v>
@@ -3386,7 +3386,7 @@
         <v>475</v>
       </c>
       <c r="O27" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="P27" t="s">
         <v>472</v>
@@ -3415,25 +3415,25 @@
         <v>0</v>
       </c>
       <c r="E28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="s">
         <v>230</v>
       </c>
       <c r="G28" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="H28" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="I28" t="s">
         <v>362</v>
       </c>
       <c r="J28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K28" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="L28" t="s">
         <v>472</v>
@@ -3448,10 +3448,10 @@
         <v>230</v>
       </c>
       <c r="P28" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="Q28" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="R28" t="s">
         <v>475</v>
@@ -3542,7 +3542,7 @@
         <v>282</v>
       </c>
       <c r="H30" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="I30" t="s">
         <v>363</v>
@@ -3557,7 +3557,7 @@
         <v>473</v>
       </c>
       <c r="M30" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="N30" t="s">
         <v>472</v>
@@ -3601,16 +3601,16 @@
         <v>252</v>
       </c>
       <c r="H31" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="I31" t="s">
         <v>364</v>
       </c>
       <c r="J31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K31" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="L31" t="s">
         <v>472</v>
@@ -3651,16 +3651,16 @@
         <v>0</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>233</v>
       </c>
       <c r="G32" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="H32" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="I32" t="s">
         <v>365</v>
@@ -3675,13 +3675,13 @@
         <v>473</v>
       </c>
       <c r="M32" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="N32" t="s">
         <v>475</v>
       </c>
       <c r="O32" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="P32" t="s">
         <v>472</v>
@@ -3690,7 +3690,7 @@
         <v>233</v>
       </c>
       <c r="R32" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S32">
         <v>1.259962577464323</v>
@@ -3719,16 +3719,16 @@
         <v>314</v>
       </c>
       <c r="H33" t="s">
-        <v>334</v>
+        <v>247</v>
       </c>
       <c r="I33" t="s">
         <v>366</v>
       </c>
       <c r="J33" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K33" t="s">
-        <v>334</v>
+        <v>247</v>
       </c>
       <c r="L33" t="s">
         <v>472</v>
@@ -3769,25 +3769,25 @@
         <v>0</v>
       </c>
       <c r="E34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="s">
         <v>235</v>
       </c>
       <c r="G34" t="s">
-        <v>297</v>
+        <v>242</v>
       </c>
       <c r="H34" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="I34" t="s">
         <v>367</v>
       </c>
       <c r="J34" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K34" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="L34" t="s">
         <v>472</v>
@@ -3799,7 +3799,7 @@
         <v>473</v>
       </c>
       <c r="O34" t="s">
-        <v>297</v>
+        <v>242</v>
       </c>
       <c r="P34" t="s">
         <v>475</v>
@@ -3808,7 +3808,7 @@
         <v>235</v>
       </c>
       <c r="R34" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S34">
         <v>1.142677885812448</v>
@@ -3887,16 +3887,16 @@
         <v>0</v>
       </c>
       <c r="E36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
         <v>236</v>
       </c>
       <c r="G36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H36" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="I36" t="s">
         <v>368</v>
@@ -3905,13 +3905,13 @@
         <v>343</v>
       </c>
       <c r="K36" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L36" t="s">
         <v>475</v>
       </c>
       <c r="M36" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="N36" t="s">
         <v>472</v>
@@ -3926,7 +3926,7 @@
         <v>236</v>
       </c>
       <c r="R36" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S36">
         <v>1.145073530222582</v>
@@ -3955,13 +3955,13 @@
         <v>289</v>
       </c>
       <c r="H37" t="s">
-        <v>268</v>
+        <v>221</v>
       </c>
       <c r="I37" t="s">
         <v>369</v>
       </c>
       <c r="J37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K37" t="s">
         <v>369</v>
@@ -3976,7 +3976,7 @@
         <v>474</v>
       </c>
       <c r="O37" t="s">
-        <v>268</v>
+        <v>221</v>
       </c>
       <c r="P37" t="s">
         <v>472</v>
@@ -4005,16 +4005,16 @@
         <v>0</v>
       </c>
       <c r="E38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="s">
         <v>238</v>
       </c>
       <c r="G38" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="H38" t="s">
-        <v>300</v>
+        <v>259</v>
       </c>
       <c r="I38" t="s">
         <v>370</v>
@@ -4023,7 +4023,7 @@
         <v>343</v>
       </c>
       <c r="K38" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="L38" t="s">
         <v>475</v>
@@ -4035,7 +4035,7 @@
         <v>473</v>
       </c>
       <c r="O38" t="s">
-        <v>300</v>
+        <v>259</v>
       </c>
       <c r="P38" t="s">
         <v>472</v>
@@ -4044,7 +4044,7 @@
         <v>238</v>
       </c>
       <c r="R38" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S38">
         <v>1.323743811417749</v>
@@ -4132,13 +4132,13 @@
         <v>229</v>
       </c>
       <c r="H40" t="s">
-        <v>323</v>
+        <v>225</v>
       </c>
       <c r="I40" t="s">
         <v>372</v>
       </c>
       <c r="J40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K40" t="s">
         <v>229</v>
@@ -4147,7 +4147,7 @@
         <v>475</v>
       </c>
       <c r="M40" t="s">
-        <v>323</v>
+        <v>225</v>
       </c>
       <c r="N40" t="s">
         <v>472</v>
@@ -4306,10 +4306,10 @@
         <v>242</v>
       </c>
       <c r="G43" t="s">
-        <v>318</v>
+        <v>249</v>
       </c>
       <c r="H43" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="I43" t="s">
         <v>374</v>
@@ -4318,7 +4318,7 @@
         <v>340</v>
       </c>
       <c r="K43" t="s">
-        <v>318</v>
+        <v>249</v>
       </c>
       <c r="L43" t="s">
         <v>475</v>
@@ -4330,7 +4330,7 @@
         <v>474</v>
       </c>
       <c r="O43" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="P43" t="s">
         <v>472</v>
@@ -4359,25 +4359,25 @@
         <v>0</v>
       </c>
       <c r="E44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
         <v>243</v>
       </c>
       <c r="G44" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
       <c r="H44" t="s">
-        <v>227</v>
+        <v>318</v>
       </c>
       <c r="I44" t="s">
         <v>375</v>
       </c>
       <c r="J44" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K44" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
       <c r="L44" t="s">
         <v>475</v>
@@ -4389,7 +4389,7 @@
         <v>473</v>
       </c>
       <c r="O44" t="s">
-        <v>227</v>
+        <v>318</v>
       </c>
       <c r="P44" t="s">
         <v>472</v>
@@ -4398,7 +4398,7 @@
         <v>243</v>
       </c>
       <c r="R44" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S44">
         <v>1.011159261895078</v>
@@ -4427,13 +4427,13 @@
         <v>228</v>
       </c>
       <c r="H45" t="s">
-        <v>222</v>
+        <v>336</v>
       </c>
       <c r="I45" t="s">
         <v>376</v>
       </c>
       <c r="J45" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K45" t="s">
         <v>244</v>
@@ -4454,7 +4454,7 @@
         <v>473</v>
       </c>
       <c r="Q45" t="s">
-        <v>222</v>
+        <v>336</v>
       </c>
       <c r="R45" t="s">
         <v>472</v>
@@ -4604,16 +4604,16 @@
         <v>327</v>
       </c>
       <c r="H48" t="s">
-        <v>337</v>
+        <v>283</v>
       </c>
       <c r="I48" t="s">
         <v>378</v>
       </c>
       <c r="J48" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="K48" t="s">
-        <v>337</v>
+        <v>283</v>
       </c>
       <c r="L48" t="s">
         <v>472</v>
@@ -4654,22 +4654,22 @@
         <v>0</v>
       </c>
       <c r="E49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
         <v>247</v>
       </c>
       <c r="G49" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
       <c r="H49" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="I49" t="s">
         <v>379</v>
       </c>
       <c r="J49" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K49" t="s">
         <v>379</v>
@@ -4681,16 +4681,16 @@
         <v>247</v>
       </c>
       <c r="N49" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O49" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="P49" t="s">
         <v>472</v>
       </c>
       <c r="Q49" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
       <c r="R49" t="s">
         <v>475</v>
@@ -4722,13 +4722,13 @@
         <v>241</v>
       </c>
       <c r="H50" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="I50" t="s">
         <v>380</v>
       </c>
       <c r="J50" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K50" t="s">
         <v>248</v>
@@ -4737,7 +4737,7 @@
         <v>474</v>
       </c>
       <c r="M50" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="N50" t="s">
         <v>472</v>
@@ -4772,22 +4772,22 @@
         <v>0</v>
       </c>
       <c r="E51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="s">
         <v>249</v>
       </c>
       <c r="G51" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="H51" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="I51" t="s">
         <v>381</v>
       </c>
       <c r="J51" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K51" t="s">
         <v>381</v>
@@ -4796,7 +4796,7 @@
         <v>473</v>
       </c>
       <c r="M51" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="N51" t="s">
         <v>472</v>
@@ -4805,10 +4805,10 @@
         <v>249</v>
       </c>
       <c r="P51" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q51" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="R51" t="s">
         <v>475</v>
@@ -4890,16 +4890,16 @@
         <v>0</v>
       </c>
       <c r="E53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
         <v>250</v>
       </c>
       <c r="G53" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="H53" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="I53" t="s">
         <v>382</v>
@@ -4911,16 +4911,16 @@
         <v>250</v>
       </c>
       <c r="L53" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M53" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="N53" t="s">
         <v>472</v>
       </c>
       <c r="O53" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="P53" t="s">
         <v>475</v>
@@ -4958,7 +4958,7 @@
         <v>261</v>
       </c>
       <c r="H54" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="I54" t="s">
         <v>383</v>
@@ -4985,7 +4985,7 @@
         <v>474</v>
       </c>
       <c r="Q54" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="R54" t="s">
         <v>472</v>
@@ -5067,22 +5067,22 @@
         <v>0</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="s">
         <v>253</v>
       </c>
       <c r="G56" t="s">
-        <v>324</v>
+        <v>223</v>
       </c>
       <c r="H56" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="I56" t="s">
         <v>385</v>
       </c>
       <c r="J56" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K56" t="s">
         <v>385</v>
@@ -5094,16 +5094,16 @@
         <v>253</v>
       </c>
       <c r="N56" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O56" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="P56" t="s">
         <v>472</v>
       </c>
       <c r="Q56" t="s">
-        <v>324</v>
+        <v>223</v>
       </c>
       <c r="R56" t="s">
         <v>475</v>
@@ -5185,22 +5185,22 @@
         <v>0</v>
       </c>
       <c r="E58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="s">
         <v>254</v>
       </c>
       <c r="G58" t="s">
-        <v>301</v>
+        <v>339</v>
       </c>
       <c r="H58" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="I58" t="s">
         <v>386</v>
       </c>
       <c r="J58" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="K58" t="s">
         <v>386</v>
@@ -5212,16 +5212,16 @@
         <v>254</v>
       </c>
       <c r="N58" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O58" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="P58" t="s">
         <v>472</v>
       </c>
       <c r="Q58" t="s">
-        <v>301</v>
+        <v>339</v>
       </c>
       <c r="R58" t="s">
         <v>475</v>
@@ -5303,16 +5303,16 @@
         <v>0</v>
       </c>
       <c r="E60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" t="s">
         <v>255</v>
       </c>
       <c r="G60" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="H60" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="I60" t="s">
         <v>387</v>
@@ -5321,13 +5321,13 @@
         <v>341</v>
       </c>
       <c r="K60" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="L60" t="s">
         <v>472</v>
       </c>
       <c r="M60" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="N60" t="s">
         <v>475</v>
@@ -5336,7 +5336,7 @@
         <v>255</v>
       </c>
       <c r="P60" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="Q60" t="s">
         <v>387</v>
@@ -5371,13 +5371,13 @@
         <v>231</v>
       </c>
       <c r="H61" t="s">
-        <v>295</v>
+        <v>233</v>
       </c>
       <c r="I61" t="s">
         <v>388</v>
       </c>
       <c r="J61" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K61" t="s">
         <v>231</v>
@@ -5386,7 +5386,7 @@
         <v>475</v>
       </c>
       <c r="M61" t="s">
-        <v>295</v>
+        <v>233</v>
       </c>
       <c r="N61" t="s">
         <v>472</v>
@@ -5430,16 +5430,16 @@
         <v>284</v>
       </c>
       <c r="H62" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I62" t="s">
         <v>389</v>
       </c>
       <c r="J62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K62" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="L62" t="s">
         <v>472</v>
@@ -5489,13 +5489,13 @@
         <v>321</v>
       </c>
       <c r="H63" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="I63" t="s">
         <v>390</v>
       </c>
       <c r="J63" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K63" t="s">
         <v>258</v>
@@ -5504,7 +5504,7 @@
         <v>474</v>
       </c>
       <c r="M63" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="N63" t="s">
         <v>472</v>
@@ -5545,19 +5545,19 @@
         <v>259</v>
       </c>
       <c r="G64" t="s">
-        <v>312</v>
+        <v>219</v>
       </c>
       <c r="H64" t="s">
-        <v>285</v>
+        <v>228</v>
       </c>
       <c r="I64" t="s">
         <v>391</v>
       </c>
       <c r="J64" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K64" t="s">
-        <v>285</v>
+        <v>228</v>
       </c>
       <c r="L64" t="s">
         <v>472</v>
@@ -5569,7 +5569,7 @@
         <v>473</v>
       </c>
       <c r="O64" t="s">
-        <v>312</v>
+        <v>219</v>
       </c>
       <c r="P64" t="s">
         <v>475</v>
@@ -5598,16 +5598,16 @@
         <v>0</v>
       </c>
       <c r="E65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" t="s">
         <v>260</v>
       </c>
       <c r="G65" t="s">
-        <v>224</v>
+        <v>305</v>
       </c>
       <c r="H65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I65" t="s">
         <v>392</v>
@@ -5619,10 +5619,10 @@
         <v>260</v>
       </c>
       <c r="L65" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N65" t="s">
         <v>472</v>
@@ -5634,7 +5634,7 @@
         <v>473</v>
       </c>
       <c r="Q65" t="s">
-        <v>224</v>
+        <v>305</v>
       </c>
       <c r="R65" t="s">
         <v>475</v>
@@ -5843,13 +5843,13 @@
         <v>316</v>
       </c>
       <c r="H69" t="s">
-        <v>225</v>
+        <v>297</v>
       </c>
       <c r="I69" t="s">
         <v>393</v>
       </c>
       <c r="J69" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K69" t="s">
         <v>261</v>
@@ -5864,7 +5864,7 @@
         <v>473</v>
       </c>
       <c r="O69" t="s">
-        <v>225</v>
+        <v>297</v>
       </c>
       <c r="P69" t="s">
         <v>472</v>
@@ -5902,13 +5902,13 @@
         <v>299</v>
       </c>
       <c r="H70" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="I70" t="s">
         <v>394</v>
       </c>
       <c r="J70" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K70" t="s">
         <v>394</v>
@@ -5929,7 +5929,7 @@
         <v>474</v>
       </c>
       <c r="Q70" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="R70" t="s">
         <v>472</v>
@@ -5958,10 +5958,10 @@
         <v>263</v>
       </c>
       <c r="G71" t="s">
-        <v>243</v>
+        <v>286</v>
       </c>
       <c r="H71" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="I71" t="s">
         <v>395</v>
@@ -5976,13 +5976,13 @@
         <v>474</v>
       </c>
       <c r="M71" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="N71" t="s">
         <v>472</v>
       </c>
       <c r="O71" t="s">
-        <v>243</v>
+        <v>286</v>
       </c>
       <c r="P71" t="s">
         <v>475</v>
@@ -6011,22 +6011,22 @@
         <v>0</v>
       </c>
       <c r="E72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
         <v>264</v>
       </c>
       <c r="G72" t="s">
-        <v>335</v>
+        <v>224</v>
       </c>
       <c r="H72" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="I72" t="s">
         <v>396</v>
       </c>
       <c r="J72" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="K72" t="s">
         <v>396</v>
@@ -6038,16 +6038,16 @@
         <v>264</v>
       </c>
       <c r="N72" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O72" t="s">
-        <v>335</v>
+        <v>224</v>
       </c>
       <c r="P72" t="s">
         <v>475</v>
       </c>
       <c r="Q72" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="R72" t="s">
         <v>472</v>
@@ -6079,13 +6079,13 @@
         <v>279</v>
       </c>
       <c r="H73" t="s">
-        <v>275</v>
+        <v>222</v>
       </c>
       <c r="I73" t="s">
         <v>397</v>
       </c>
       <c r="J73" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K73" t="s">
         <v>279</v>
@@ -6094,7 +6094,7 @@
         <v>475</v>
       </c>
       <c r="M73" t="s">
-        <v>275</v>
+        <v>222</v>
       </c>
       <c r="N73" t="s">
         <v>472</v>
@@ -6138,13 +6138,13 @@
         <v>276</v>
       </c>
       <c r="H74" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="I74" t="s">
         <v>398</v>
       </c>
       <c r="J74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K74" t="s">
         <v>276</v>
@@ -6153,7 +6153,7 @@
         <v>475</v>
       </c>
       <c r="M74" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="N74" t="s">
         <v>472</v>
@@ -6256,7 +6256,7 @@
         <v>266</v>
       </c>
       <c r="H76" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="I76" t="s">
         <v>399</v>
@@ -6271,7 +6271,7 @@
         <v>474</v>
       </c>
       <c r="M76" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="N76" t="s">
         <v>472</v>
@@ -6306,22 +6306,22 @@
         <v>0</v>
       </c>
       <c r="E77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="s">
         <v>268</v>
       </c>
       <c r="G77" t="s">
-        <v>333</v>
+        <v>247</v>
       </c>
       <c r="H77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I77" t="s">
         <v>400</v>
       </c>
       <c r="J77" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K77" t="s">
         <v>400</v>
@@ -6330,13 +6330,13 @@
         <v>473</v>
       </c>
       <c r="M77" t="s">
-        <v>333</v>
+        <v>247</v>
       </c>
       <c r="N77" t="s">
         <v>475</v>
       </c>
       <c r="O77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P77" t="s">
         <v>472</v>
@@ -6345,7 +6345,7 @@
         <v>268</v>
       </c>
       <c r="R77" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S77">
         <v>1.080503952536192</v>
@@ -6489,10 +6489,10 @@
         <v>269</v>
       </c>
       <c r="G80" t="s">
-        <v>300</v>
+        <v>222</v>
       </c>
       <c r="H80" t="s">
-        <v>211</v>
+        <v>321</v>
       </c>
       <c r="I80" t="s">
         <v>401</v>
@@ -6507,13 +6507,13 @@
         <v>473</v>
       </c>
       <c r="M80" t="s">
-        <v>300</v>
+        <v>222</v>
       </c>
       <c r="N80" t="s">
         <v>475</v>
       </c>
       <c r="O80" t="s">
-        <v>211</v>
+        <v>321</v>
       </c>
       <c r="P80" t="s">
         <v>472</v>
@@ -6542,16 +6542,16 @@
         <v>0</v>
       </c>
       <c r="E81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="s">
         <v>270</v>
       </c>
       <c r="G81" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H81" t="s">
-        <v>272</v>
+        <v>316</v>
       </c>
       <c r="I81" t="s">
         <v>402</v>
@@ -6560,7 +6560,7 @@
         <v>340</v>
       </c>
       <c r="K81" t="s">
-        <v>272</v>
+        <v>316</v>
       </c>
       <c r="L81" t="s">
         <v>472</v>
@@ -6572,7 +6572,7 @@
         <v>473</v>
       </c>
       <c r="O81" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="P81" t="s">
         <v>475</v>
@@ -6581,7 +6581,7 @@
         <v>270</v>
       </c>
       <c r="R81" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S81">
         <v>1.053608001125836</v>
@@ -6610,13 +6610,13 @@
         <v>294</v>
       </c>
       <c r="H82" t="s">
-        <v>223</v>
+        <v>303</v>
       </c>
       <c r="I82" t="s">
         <v>403</v>
       </c>
       <c r="J82" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K82" t="s">
         <v>403</v>
@@ -6631,7 +6631,7 @@
         <v>474</v>
       </c>
       <c r="O82" t="s">
-        <v>223</v>
+        <v>303</v>
       </c>
       <c r="P82" t="s">
         <v>472</v>
@@ -6669,16 +6669,16 @@
         <v>258</v>
       </c>
       <c r="H83" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="I83" t="s">
         <v>404</v>
       </c>
       <c r="J83" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="K83" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="L83" t="s">
         <v>472</v>
@@ -6719,16 +6719,16 @@
         <v>0</v>
       </c>
       <c r="E84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="s">
         <v>273</v>
       </c>
       <c r="G84" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="H84" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
       <c r="I84" t="s">
         <v>405</v>
@@ -6740,16 +6740,16 @@
         <v>273</v>
       </c>
       <c r="L84" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M84" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="N84" t="s">
         <v>475</v>
       </c>
       <c r="O84" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
       <c r="P84" t="s">
         <v>472</v>
@@ -6837,37 +6837,37 @@
         <v>0</v>
       </c>
       <c r="E86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
         <v>274</v>
       </c>
       <c r="G86" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
       <c r="H86" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="I86" t="s">
         <v>406</v>
       </c>
       <c r="J86" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K86" t="s">
         <v>274</v>
       </c>
       <c r="L86" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M86" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="N86" t="s">
         <v>472</v>
       </c>
       <c r="O86" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
       <c r="P86" t="s">
         <v>475</v>
@@ -6896,16 +6896,16 @@
         <v>0</v>
       </c>
       <c r="E87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" t="s">
         <v>275</v>
       </c>
       <c r="G87" t="s">
-        <v>221</v>
+        <v>318</v>
       </c>
       <c r="H87" t="s">
-        <v>299</v>
+        <v>232</v>
       </c>
       <c r="I87" t="s">
         <v>407</v>
@@ -6920,13 +6920,13 @@
         <v>473</v>
       </c>
       <c r="M87" t="s">
-        <v>299</v>
+        <v>232</v>
       </c>
       <c r="N87" t="s">
         <v>472</v>
       </c>
       <c r="O87" t="s">
-        <v>221</v>
+        <v>318</v>
       </c>
       <c r="P87" t="s">
         <v>475</v>
@@ -6935,7 +6935,7 @@
         <v>275</v>
       </c>
       <c r="R87" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S87">
         <v>1.070444878025286</v>
@@ -6964,7 +6964,7 @@
         <v>257</v>
       </c>
       <c r="H88" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="I88" t="s">
         <v>408</v>
@@ -6985,7 +6985,7 @@
         <v>474</v>
       </c>
       <c r="O88" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="P88" t="s">
         <v>472</v>
@@ -7014,31 +7014,31 @@
         <v>0</v>
       </c>
       <c r="E89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" t="s">
         <v>277</v>
       </c>
       <c r="G89" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="H89" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="I89" t="s">
         <v>409</v>
       </c>
       <c r="J89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K89" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="L89" t="s">
         <v>475</v>
       </c>
       <c r="M89" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="N89" t="s">
         <v>472</v>
@@ -7047,7 +7047,7 @@
         <v>277</v>
       </c>
       <c r="P89" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="Q89" t="s">
         <v>409</v>
@@ -7197,16 +7197,16 @@
         <v>278</v>
       </c>
       <c r="G92" t="s">
-        <v>336</v>
+        <v>221</v>
       </c>
       <c r="H92" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="I92" t="s">
         <v>410</v>
       </c>
       <c r="J92" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="K92" t="s">
         <v>278</v>
@@ -7215,7 +7215,7 @@
         <v>476</v>
       </c>
       <c r="M92" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="N92" t="s">
         <v>472</v>
@@ -7227,7 +7227,7 @@
         <v>473</v>
       </c>
       <c r="Q92" t="s">
-        <v>336</v>
+        <v>221</v>
       </c>
       <c r="R92" t="s">
         <v>475</v>
@@ -7309,25 +7309,25 @@
         <v>0</v>
       </c>
       <c r="E94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" t="s">
         <v>280</v>
       </c>
       <c r="G94" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H94" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="I94" t="s">
         <v>412</v>
       </c>
       <c r="J94" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K94" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="L94" t="s">
         <v>475</v>
@@ -7336,7 +7336,7 @@
         <v>280</v>
       </c>
       <c r="N94" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O94" t="s">
         <v>412</v>
@@ -7345,7 +7345,7 @@
         <v>473</v>
       </c>
       <c r="Q94" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="R94" t="s">
         <v>472</v>
@@ -7377,7 +7377,7 @@
         <v>302</v>
       </c>
       <c r="H95" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="I95" t="s">
         <v>413</v>
@@ -7398,7 +7398,7 @@
         <v>475</v>
       </c>
       <c r="O95" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="P95" t="s">
         <v>472</v>
@@ -7554,13 +7554,13 @@
         <v>239</v>
       </c>
       <c r="H98" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="I98" t="s">
         <v>414</v>
       </c>
       <c r="J98" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K98" t="s">
         <v>414</v>
@@ -7575,7 +7575,7 @@
         <v>475</v>
       </c>
       <c r="O98" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="P98" t="s">
         <v>472</v>
@@ -7604,37 +7604,37 @@
         <v>0</v>
       </c>
       <c r="E99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" t="s">
         <v>283</v>
       </c>
       <c r="G99" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H99" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I99" t="s">
         <v>415</v>
       </c>
       <c r="J99" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K99" t="s">
         <v>283</v>
       </c>
       <c r="L99" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M99" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="N99" t="s">
         <v>475</v>
       </c>
       <c r="O99" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="P99" t="s">
         <v>472</v>
@@ -7731,13 +7731,13 @@
         <v>313</v>
       </c>
       <c r="H101" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I101" t="s">
         <v>416</v>
       </c>
       <c r="J101" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K101" t="s">
         <v>416</v>
@@ -7758,7 +7758,7 @@
         <v>475</v>
       </c>
       <c r="Q101" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="R101" t="s">
         <v>472</v>
@@ -7790,13 +7790,13 @@
         <v>317</v>
       </c>
       <c r="H102" t="s">
-        <v>320</v>
+        <v>254</v>
       </c>
       <c r="I102" t="s">
         <v>417</v>
       </c>
       <c r="J102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K102" t="s">
         <v>317</v>
@@ -7817,7 +7817,7 @@
         <v>474</v>
       </c>
       <c r="Q102" t="s">
-        <v>320</v>
+        <v>254</v>
       </c>
       <c r="R102" t="s">
         <v>472</v>
@@ -7840,25 +7840,25 @@
         <v>0</v>
       </c>
       <c r="E103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" t="s">
         <v>286</v>
       </c>
       <c r="G103" t="s">
-        <v>277</v>
+        <v>333</v>
       </c>
       <c r="H103" t="s">
-        <v>218</v>
+        <v>317</v>
       </c>
       <c r="I103" t="s">
         <v>418</v>
       </c>
       <c r="J103" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K103" t="s">
-        <v>218</v>
+        <v>317</v>
       </c>
       <c r="L103" t="s">
         <v>472</v>
@@ -7867,10 +7867,10 @@
         <v>286</v>
       </c>
       <c r="N103" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O103" t="s">
-        <v>277</v>
+        <v>333</v>
       </c>
       <c r="P103" t="s">
         <v>475</v>
@@ -7958,16 +7958,16 @@
         <v>0</v>
       </c>
       <c r="E105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" t="s">
         <v>288</v>
       </c>
       <c r="G105" t="s">
-        <v>253</v>
+        <v>297</v>
       </c>
       <c r="H105" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="I105" t="s">
         <v>420</v>
@@ -7976,13 +7976,13 @@
         <v>340</v>
       </c>
       <c r="K105" t="s">
-        <v>253</v>
+        <v>297</v>
       </c>
       <c r="L105" t="s">
         <v>475</v>
       </c>
       <c r="M105" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="N105" t="s">
         <v>472</v>
@@ -7991,7 +7991,7 @@
         <v>288</v>
       </c>
       <c r="P105" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q105" t="s">
         <v>420</v>
@@ -8026,13 +8026,13 @@
         <v>212</v>
       </c>
       <c r="H106" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="I106" t="s">
         <v>421</v>
       </c>
       <c r="J106" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K106" t="s">
         <v>421</v>
@@ -8047,7 +8047,7 @@
         <v>474</v>
       </c>
       <c r="O106" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="P106" t="s">
         <v>472</v>
@@ -8203,7 +8203,7 @@
         <v>275</v>
       </c>
       <c r="H109" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
       <c r="I109" t="s">
         <v>422</v>
@@ -8230,7 +8230,7 @@
         <v>475</v>
       </c>
       <c r="Q109" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
       <c r="R109" t="s">
         <v>472</v>
@@ -8312,25 +8312,25 @@
         <v>0</v>
       </c>
       <c r="E111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F111" t="s">
         <v>291</v>
       </c>
       <c r="G111" t="s">
-        <v>220</v>
+        <v>283</v>
       </c>
       <c r="H111" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
       <c r="I111" t="s">
         <v>423</v>
       </c>
       <c r="J111" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K111" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
       <c r="L111" t="s">
         <v>472</v>
@@ -8342,7 +8342,7 @@
         <v>473</v>
       </c>
       <c r="O111" t="s">
-        <v>220</v>
+        <v>283</v>
       </c>
       <c r="P111" t="s">
         <v>475</v>
@@ -8351,7 +8351,7 @@
         <v>291</v>
       </c>
       <c r="R111" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S111">
         <v>1.118577695525584</v>
@@ -8371,31 +8371,31 @@
         <v>0</v>
       </c>
       <c r="E112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112" t="s">
         <v>292</v>
       </c>
       <c r="G112" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="H112" t="s">
-        <v>221</v>
+        <v>285</v>
       </c>
       <c r="I112" t="s">
         <v>424</v>
       </c>
       <c r="J112" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K112" t="s">
         <v>292</v>
       </c>
       <c r="L112" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M112" t="s">
-        <v>221</v>
+        <v>285</v>
       </c>
       <c r="N112" t="s">
         <v>472</v>
@@ -8407,7 +8407,7 @@
         <v>473</v>
       </c>
       <c r="Q112" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="R112" t="s">
         <v>475</v>
@@ -8548,31 +8548,31 @@
         <v>0</v>
       </c>
       <c r="E115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F115" t="s">
         <v>293</v>
       </c>
       <c r="G115" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H115" t="s">
-        <v>267</v>
+        <v>326</v>
       </c>
       <c r="I115" t="s">
         <v>425</v>
       </c>
       <c r="J115" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="K115" t="s">
-        <v>267</v>
+        <v>326</v>
       </c>
       <c r="L115" t="s">
         <v>472</v>
       </c>
       <c r="M115" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N115" t="s">
         <v>475</v>
@@ -8587,7 +8587,7 @@
         <v>293</v>
       </c>
       <c r="R115" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S115">
         <v>1.082831592752383</v>
@@ -8675,13 +8675,13 @@
         <v>240</v>
       </c>
       <c r="H117" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="I117" t="s">
         <v>426</v>
       </c>
       <c r="J117" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K117" t="s">
         <v>426</v>
@@ -8696,7 +8696,7 @@
         <v>474</v>
       </c>
       <c r="O117" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="P117" t="s">
         <v>472</v>
@@ -8843,37 +8843,37 @@
         <v>0</v>
       </c>
       <c r="E120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F120" t="s">
         <v>295</v>
       </c>
       <c r="G120" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H120" t="s">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="I120" t="s">
         <v>427</v>
       </c>
       <c r="J120" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="K120" t="s">
         <v>295</v>
       </c>
       <c r="L120" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M120" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N120" t="s">
         <v>475</v>
       </c>
       <c r="O120" t="s">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="P120" t="s">
         <v>472</v>
@@ -8911,13 +8911,13 @@
         <v>311</v>
       </c>
       <c r="H121" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I121" t="s">
         <v>428</v>
       </c>
       <c r="J121" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K121" t="s">
         <v>296</v>
@@ -8938,7 +8938,7 @@
         <v>475</v>
       </c>
       <c r="Q121" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="R121" t="s">
         <v>472</v>
@@ -9138,25 +9138,25 @@
         <v>0</v>
       </c>
       <c r="E125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F125" t="s">
         <v>297</v>
       </c>
       <c r="G125" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H125" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="I125" t="s">
         <v>429</v>
       </c>
       <c r="J125" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K125" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="L125" t="s">
         <v>472</v>
@@ -9165,10 +9165,10 @@
         <v>297</v>
       </c>
       <c r="N125" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O125" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="P125" t="s">
         <v>475</v>
@@ -9324,13 +9324,13 @@
         <v>325</v>
       </c>
       <c r="H128" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="I128" t="s">
         <v>430</v>
       </c>
       <c r="J128" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K128" t="s">
         <v>325</v>
@@ -9351,7 +9351,7 @@
         <v>473</v>
       </c>
       <c r="Q128" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="R128" t="s">
         <v>472</v>
@@ -9383,13 +9383,13 @@
         <v>256</v>
       </c>
       <c r="H129" t="s">
-        <v>304</v>
+        <v>223</v>
       </c>
       <c r="I129" t="s">
         <v>431</v>
       </c>
       <c r="J129" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K129" t="s">
         <v>256</v>
@@ -9410,7 +9410,7 @@
         <v>473</v>
       </c>
       <c r="Q129" t="s">
-        <v>304</v>
+        <v>223</v>
       </c>
       <c r="R129" t="s">
         <v>472</v>
@@ -9433,13 +9433,13 @@
         <v>0</v>
       </c>
       <c r="E130" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F130" t="s">
         <v>300</v>
       </c>
       <c r="G130" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="H130" t="s">
         <v>307</v>
@@ -9460,7 +9460,7 @@
         <v>300</v>
       </c>
       <c r="N130" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O130" t="s">
         <v>307</v>
@@ -9469,7 +9469,7 @@
         <v>472</v>
       </c>
       <c r="Q130" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="R130" t="s">
         <v>475</v>
@@ -9551,25 +9551,25 @@
         <v>0</v>
       </c>
       <c r="E132" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132" t="s">
         <v>301</v>
       </c>
       <c r="G132" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="H132" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="I132" t="s">
         <v>433</v>
       </c>
       <c r="J132" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K132" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="L132" t="s">
         <v>472</v>
@@ -9581,7 +9581,7 @@
         <v>473</v>
       </c>
       <c r="O132" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="P132" t="s">
         <v>475</v>
@@ -9590,7 +9590,7 @@
         <v>301</v>
       </c>
       <c r="R132" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S132">
         <v>1.016034106086119</v>
@@ -9678,16 +9678,16 @@
         <v>211</v>
       </c>
       <c r="H134" t="s">
-        <v>339</v>
+        <v>286</v>
       </c>
       <c r="I134" t="s">
         <v>434</v>
       </c>
       <c r="J134" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K134" t="s">
-        <v>339</v>
+        <v>286</v>
       </c>
       <c r="L134" t="s">
         <v>472</v>
@@ -9787,28 +9787,28 @@
         <v>0</v>
       </c>
       <c r="E136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F136" t="s">
         <v>303</v>
       </c>
       <c r="G136" t="s">
-        <v>250</v>
+        <v>312</v>
       </c>
       <c r="H136" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="I136" t="s">
         <v>435</v>
       </c>
       <c r="J136" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K136" t="s">
         <v>303</v>
       </c>
       <c r="L136" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M136" t="s">
         <v>435</v>
@@ -9817,13 +9817,13 @@
         <v>473</v>
       </c>
       <c r="O136" t="s">
-        <v>250</v>
+        <v>312</v>
       </c>
       <c r="P136" t="s">
         <v>475</v>
       </c>
       <c r="Q136" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="R136" t="s">
         <v>472</v>
@@ -9846,16 +9846,16 @@
         <v>0</v>
       </c>
       <c r="E137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" t="s">
         <v>304</v>
       </c>
       <c r="G137" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="H137" t="s">
-        <v>249</v>
+        <v>301</v>
       </c>
       <c r="I137" t="s">
         <v>436</v>
@@ -9870,13 +9870,13 @@
         <v>473</v>
       </c>
       <c r="M137" t="s">
-        <v>249</v>
+        <v>301</v>
       </c>
       <c r="N137" t="s">
         <v>472</v>
       </c>
       <c r="O137" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="P137" t="s">
         <v>475</v>
@@ -9885,7 +9885,7 @@
         <v>304</v>
       </c>
       <c r="R137" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S137">
         <v>1.013820989571717</v>
@@ -9964,25 +9964,25 @@
         <v>0</v>
       </c>
       <c r="E139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="s">
         <v>305</v>
       </c>
       <c r="G139" t="s">
-        <v>218</v>
+        <v>301</v>
       </c>
       <c r="H139" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="I139" t="s">
         <v>437</v>
       </c>
       <c r="J139" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K139" t="s">
-        <v>218</v>
+        <v>301</v>
       </c>
       <c r="L139" t="s">
         <v>475</v>
@@ -9991,7 +9991,7 @@
         <v>305</v>
       </c>
       <c r="N139" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O139" t="s">
         <v>437</v>
@@ -10000,7 +10000,7 @@
         <v>473</v>
       </c>
       <c r="Q139" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="R139" t="s">
         <v>472</v>
@@ -10091,13 +10091,13 @@
         <v>315</v>
       </c>
       <c r="H141" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="I141" t="s">
         <v>438</v>
       </c>
       <c r="J141" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K141" t="s">
         <v>315</v>
@@ -10118,7 +10118,7 @@
         <v>474</v>
       </c>
       <c r="Q141" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="R141" t="s">
         <v>472</v>
@@ -10259,25 +10259,25 @@
         <v>0</v>
       </c>
       <c r="E144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F144" t="s">
         <v>307</v>
       </c>
       <c r="G144" t="s">
-        <v>236</v>
+        <v>336</v>
       </c>
       <c r="H144" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="I144" t="s">
         <v>439</v>
       </c>
       <c r="J144" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="K144" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="L144" t="s">
         <v>472</v>
@@ -10286,10 +10286,10 @@
         <v>307</v>
       </c>
       <c r="N144" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O144" t="s">
-        <v>236</v>
+        <v>336</v>
       </c>
       <c r="P144" t="s">
         <v>475</v>
@@ -10318,22 +10318,22 @@
         <v>0</v>
       </c>
       <c r="E145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F145" t="s">
         <v>308</v>
       </c>
       <c r="G145" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="H145" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="I145" t="s">
         <v>440</v>
       </c>
       <c r="J145" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K145" t="s">
         <v>440</v>
@@ -10342,7 +10342,7 @@
         <v>473</v>
       </c>
       <c r="M145" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="N145" t="s">
         <v>472</v>
@@ -10351,10 +10351,10 @@
         <v>308</v>
       </c>
       <c r="P145" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q145" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="R145" t="s">
         <v>475</v>
@@ -10445,13 +10445,13 @@
         <v>337</v>
       </c>
       <c r="H147" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
       <c r="I147" t="s">
         <v>441</v>
       </c>
       <c r="J147" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K147" t="s">
         <v>309</v>
@@ -10466,7 +10466,7 @@
         <v>473</v>
       </c>
       <c r="O147" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
       <c r="P147" t="s">
         <v>472</v>
@@ -10504,16 +10504,16 @@
         <v>232</v>
       </c>
       <c r="H148" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="I148" t="s">
         <v>442</v>
       </c>
       <c r="J148" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K148" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="L148" t="s">
         <v>472</v>
@@ -10622,7 +10622,7 @@
         <v>246</v>
       </c>
       <c r="H150" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="I150" t="s">
         <v>443</v>
@@ -10637,7 +10637,7 @@
         <v>474</v>
       </c>
       <c r="M150" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="N150" t="s">
         <v>472</v>
@@ -10672,25 +10672,25 @@
         <v>0</v>
       </c>
       <c r="E151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F151" t="s">
         <v>312</v>
       </c>
       <c r="G151" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="H151" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="I151" t="s">
         <v>444</v>
       </c>
       <c r="J151" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K151" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="L151" t="s">
         <v>472</v>
@@ -10699,7 +10699,7 @@
         <v>312</v>
       </c>
       <c r="N151" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O151" t="s">
         <v>444</v>
@@ -10708,7 +10708,7 @@
         <v>473</v>
       </c>
       <c r="Q151" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="R151" t="s">
         <v>475</v>
@@ -10799,7 +10799,7 @@
         <v>329</v>
       </c>
       <c r="H153" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="I153" t="s">
         <v>445</v>
@@ -10814,7 +10814,7 @@
         <v>474</v>
       </c>
       <c r="M153" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="N153" t="s">
         <v>472</v>
@@ -10858,13 +10858,13 @@
         <v>215</v>
       </c>
       <c r="H154" t="s">
-        <v>324</v>
+        <v>220</v>
       </c>
       <c r="I154" t="s">
         <v>446</v>
       </c>
       <c r="J154" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K154" t="s">
         <v>446</v>
@@ -10885,7 +10885,7 @@
         <v>475</v>
       </c>
       <c r="Q154" t="s">
-        <v>324</v>
+        <v>220</v>
       </c>
       <c r="R154" t="s">
         <v>472</v>
@@ -10976,13 +10976,13 @@
         <v>306</v>
       </c>
       <c r="H156" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="I156" t="s">
         <v>447</v>
       </c>
       <c r="J156" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K156" t="s">
         <v>315</v>
@@ -11003,7 +11003,7 @@
         <v>473</v>
       </c>
       <c r="Q156" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="R156" t="s">
         <v>472</v>
@@ -11035,7 +11035,7 @@
         <v>217</v>
       </c>
       <c r="H157" t="s">
-        <v>331</v>
+        <v>244</v>
       </c>
       <c r="I157" t="s">
         <v>448</v>
@@ -11050,7 +11050,7 @@
         <v>475</v>
       </c>
       <c r="M157" t="s">
-        <v>331</v>
+        <v>244</v>
       </c>
       <c r="N157" t="s">
         <v>472</v>
@@ -11153,13 +11153,13 @@
         <v>285</v>
       </c>
       <c r="H159" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="I159" t="s">
         <v>449</v>
       </c>
       <c r="J159" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K159" t="s">
         <v>317</v>
@@ -11174,7 +11174,7 @@
         <v>475</v>
       </c>
       <c r="O159" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="P159" t="s">
         <v>472</v>
@@ -11203,25 +11203,25 @@
         <v>0</v>
       </c>
       <c r="E160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F160" t="s">
         <v>318</v>
       </c>
       <c r="G160" t="s">
-        <v>280</v>
+        <v>218</v>
       </c>
       <c r="H160" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="I160" t="s">
         <v>450</v>
       </c>
       <c r="J160" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="K160" t="s">
-        <v>280</v>
+        <v>218</v>
       </c>
       <c r="L160" t="s">
         <v>475</v>
@@ -11230,10 +11230,10 @@
         <v>318</v>
       </c>
       <c r="N160" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O160" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="P160" t="s">
         <v>472</v>
@@ -11262,31 +11262,31 @@
         <v>0</v>
       </c>
       <c r="E161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F161" t="s">
         <v>319</v>
       </c>
       <c r="G161" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="H161" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="I161" t="s">
         <v>451</v>
       </c>
       <c r="J161" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K161" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="L161" t="s">
         <v>472</v>
       </c>
       <c r="M161" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="N161" t="s">
         <v>475</v>
@@ -11295,7 +11295,7 @@
         <v>319</v>
       </c>
       <c r="P161" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q161" t="s">
         <v>451</v>
@@ -11498,16 +11498,16 @@
         <v>0</v>
       </c>
       <c r="E165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F165" t="s">
         <v>320</v>
       </c>
       <c r="G165" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="H165" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
       <c r="I165" t="s">
         <v>452</v>
@@ -11525,16 +11525,16 @@
         <v>320</v>
       </c>
       <c r="N165" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O165" t="s">
-        <v>253</v>
+        <v>339</v>
       </c>
       <c r="P165" t="s">
         <v>472</v>
       </c>
       <c r="Q165" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="R165" t="s">
         <v>475</v>
@@ -11684,13 +11684,13 @@
         <v>214</v>
       </c>
       <c r="H168" t="s">
-        <v>262</v>
+        <v>335</v>
       </c>
       <c r="I168" t="s">
         <v>453</v>
       </c>
       <c r="J168" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K168" t="s">
         <v>321</v>
@@ -11699,7 +11699,7 @@
         <v>474</v>
       </c>
       <c r="M168" t="s">
-        <v>262</v>
+        <v>335</v>
       </c>
       <c r="N168" t="s">
         <v>472</v>
@@ -11734,16 +11734,16 @@
         <v>0</v>
       </c>
       <c r="E169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F169" t="s">
         <v>322</v>
       </c>
       <c r="G169" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
       <c r="H169" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="I169" t="s">
         <v>454</v>
@@ -11758,13 +11758,13 @@
         <v>473</v>
       </c>
       <c r="M169" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
       <c r="N169" t="s">
         <v>475</v>
       </c>
       <c r="O169" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="P169" t="s">
         <v>472</v>
@@ -11773,7 +11773,7 @@
         <v>322</v>
       </c>
       <c r="R169" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S169">
         <v>1.243073535619158</v>
@@ -11858,16 +11858,16 @@
         <v>323</v>
       </c>
       <c r="G171" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="H171" t="s">
-        <v>214</v>
+        <v>338</v>
       </c>
       <c r="I171" t="s">
         <v>455</v>
       </c>
       <c r="J171" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K171" t="s">
         <v>455</v>
@@ -11876,13 +11876,13 @@
         <v>473</v>
       </c>
       <c r="M171" t="s">
-        <v>214</v>
+        <v>338</v>
       </c>
       <c r="N171" t="s">
         <v>472</v>
       </c>
       <c r="O171" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="P171" t="s">
         <v>475</v>
@@ -11911,22 +11911,22 @@
         <v>0</v>
       </c>
       <c r="E172" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F172" t="s">
         <v>324</v>
       </c>
       <c r="G172" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="H172" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="I172" t="s">
         <v>456</v>
       </c>
       <c r="J172" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K172" t="s">
         <v>456</v>
@@ -11935,7 +11935,7 @@
         <v>473</v>
       </c>
       <c r="M172" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="N172" t="s">
         <v>472</v>
@@ -11944,10 +11944,10 @@
         <v>324</v>
       </c>
       <c r="P172" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q172" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="R172" t="s">
         <v>475</v>
@@ -11979,13 +11979,13 @@
         <v>267</v>
       </c>
       <c r="H173" t="s">
-        <v>236</v>
+        <v>330</v>
       </c>
       <c r="I173" t="s">
         <v>457</v>
       </c>
       <c r="J173" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K173" t="s">
         <v>457</v>
@@ -11994,7 +11994,7 @@
         <v>473</v>
       </c>
       <c r="M173" t="s">
-        <v>236</v>
+        <v>330</v>
       </c>
       <c r="N173" t="s">
         <v>472</v>
@@ -12088,31 +12088,31 @@
         <v>0</v>
       </c>
       <c r="E175" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F175" t="s">
         <v>326</v>
       </c>
       <c r="G175" t="s">
-        <v>235</v>
+        <v>278</v>
       </c>
       <c r="H175" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="I175" t="s">
         <v>458</v>
       </c>
       <c r="J175" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K175" t="s">
-        <v>235</v>
+        <v>278</v>
       </c>
       <c r="L175" t="s">
         <v>475</v>
       </c>
       <c r="M175" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="N175" t="s">
         <v>472</v>
@@ -12127,7 +12127,7 @@
         <v>326</v>
       </c>
       <c r="R175" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S175">
         <v>1.119437725646427</v>
@@ -12156,13 +12156,13 @@
         <v>281</v>
       </c>
       <c r="H176" t="s">
-        <v>238</v>
+        <v>322</v>
       </c>
       <c r="I176" t="s">
         <v>459</v>
       </c>
       <c r="J176" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K176" t="s">
         <v>327</v>
@@ -12183,7 +12183,7 @@
         <v>475</v>
       </c>
       <c r="Q176" t="s">
-        <v>238</v>
+        <v>322</v>
       </c>
       <c r="R176" t="s">
         <v>472</v>
@@ -12265,25 +12265,25 @@
         <v>0</v>
       </c>
       <c r="E178" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F178" t="s">
         <v>328</v>
       </c>
       <c r="G178" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="H178" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="I178" t="s">
         <v>460</v>
       </c>
       <c r="J178" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K178" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="L178" t="s">
         <v>472</v>
@@ -12292,7 +12292,7 @@
         <v>328</v>
       </c>
       <c r="N178" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="O178" t="s">
         <v>460</v>
@@ -12301,7 +12301,7 @@
         <v>473</v>
       </c>
       <c r="Q178" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="R178" t="s">
         <v>475</v>
@@ -12333,7 +12333,7 @@
         <v>272</v>
       </c>
       <c r="H179" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="I179" t="s">
         <v>461</v>
@@ -12360,7 +12360,7 @@
         <v>475</v>
       </c>
       <c r="Q179" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="R179" t="s">
         <v>472</v>
@@ -12451,13 +12451,13 @@
         <v>248</v>
       </c>
       <c r="H181" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="I181" t="s">
         <v>463</v>
       </c>
       <c r="J181" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K181" t="s">
         <v>331</v>
@@ -12472,7 +12472,7 @@
         <v>473</v>
       </c>
       <c r="O181" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="P181" t="s">
         <v>472</v>
@@ -12619,16 +12619,16 @@
         <v>0</v>
       </c>
       <c r="E184" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F184" t="s">
         <v>332</v>
       </c>
       <c r="G184" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="H184" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I184" t="s">
         <v>464</v>
@@ -12637,7 +12637,7 @@
         <v>343</v>
       </c>
       <c r="K184" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="L184" t="s">
         <v>475</v>
@@ -12652,10 +12652,10 @@
         <v>332</v>
       </c>
       <c r="P184" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="Q184" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="R184" t="s">
         <v>472</v>
@@ -12684,25 +12684,25 @@
         <v>333</v>
       </c>
       <c r="G185" t="s">
-        <v>308</v>
+        <v>220</v>
       </c>
       <c r="H185" t="s">
-        <v>325</v>
+        <v>241</v>
       </c>
       <c r="I185" t="s">
         <v>465</v>
       </c>
       <c r="J185" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K185" t="s">
-        <v>308</v>
+        <v>220</v>
       </c>
       <c r="L185" t="s">
         <v>475</v>
       </c>
       <c r="M185" t="s">
-        <v>325</v>
+        <v>241</v>
       </c>
       <c r="N185" t="s">
         <v>472</v>
@@ -12737,13 +12737,13 @@
         <v>0</v>
       </c>
       <c r="E186" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F186" t="s">
         <v>334</v>
       </c>
       <c r="G186" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="H186" t="s">
         <v>216</v>
@@ -12758,10 +12758,10 @@
         <v>334</v>
       </c>
       <c r="L186" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M186" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="N186" t="s">
         <v>475</v>
@@ -12855,16 +12855,16 @@
         <v>0</v>
       </c>
       <c r="E188" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F188" t="s">
         <v>335</v>
       </c>
       <c r="G188" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="H188" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
       <c r="I188" t="s">
         <v>467</v>
@@ -12879,13 +12879,13 @@
         <v>473</v>
       </c>
       <c r="M188" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
       <c r="N188" t="s">
         <v>472</v>
       </c>
       <c r="O188" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="P188" t="s">
         <v>475</v>
@@ -12894,7 +12894,7 @@
         <v>335</v>
       </c>
       <c r="R188" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="S188">
         <v>1.003033753569337</v>
@@ -12914,25 +12914,25 @@
         <v>0</v>
       </c>
       <c r="E189" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F189" t="s">
         <v>336</v>
       </c>
       <c r="G189" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="H189" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="I189" t="s">
         <v>468</v>
       </c>
       <c r="J189" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="K189" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="L189" t="s">
         <v>475</v>
@@ -12944,7 +12944,7 @@
         <v>473</v>
       </c>
       <c r="O189" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="P189" t="s">
         <v>472</v>
@@ -12953,7 +12953,7 @@
         <v>336</v>
       </c>
       <c r="R189" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S189">
         <v>1.023510474767011</v>
@@ -12982,13 +12982,13 @@
         <v>265</v>
       </c>
       <c r="H190" t="s">
-        <v>322</v>
+        <v>264</v>
       </c>
       <c r="I190" t="s">
         <v>469</v>
       </c>
       <c r="J190" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K190" t="s">
         <v>469</v>
@@ -13003,7 +13003,7 @@
         <v>474</v>
       </c>
       <c r="O190" t="s">
-        <v>322</v>
+        <v>264</v>
       </c>
       <c r="P190" t="s">
         <v>472</v>
@@ -13150,22 +13150,22 @@
         <v>0</v>
       </c>
       <c r="E193" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F193" t="s">
         <v>339</v>
       </c>
       <c r="G193" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="H193" t="s">
-        <v>302</v>
+        <v>337</v>
       </c>
       <c r="I193" t="s">
         <v>471</v>
       </c>
       <c r="J193" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K193" t="s">
         <v>471</v>
@@ -13177,16 +13177,16 @@
         <v>339</v>
       </c>
       <c r="N193" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O193" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="P193" t="s">
         <v>475</v>
       </c>
       <c r="Q193" t="s">
-        <v>302</v>
+        <v>337</v>
       </c>
       <c r="R193" t="s">
         <v>472</v>

</xml_diff>